<commit_message>
Working repo. Update to doc about the datamodels.
</commit_message>
<xml_diff>
--- a/docs/Favit_DataModel.xlsx
+++ b/docs/Favit_DataModel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Damola\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\company\Company_Projects\FavitApp\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
   <si>
     <t xml:space="preserve">User </t>
   </si>
@@ -177,6 +177,21 @@
   </si>
   <si>
     <t>OccasionId</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>ModoMembershipDate</t>
+  </si>
+  <si>
+    <t>RegCode</t>
+  </si>
+  <si>
+    <t>CardOnFile</t>
   </si>
 </sst>
 </file>
@@ -556,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,12 +586,12 @@
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -595,8 +610,23 @@
       <c r="F2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -616,7 +646,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -636,7 +666,7 @@
         <v>41708</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -656,12 +686,12 @@
         <v>41920</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -669,7 +699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -677,7 +707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>2</v>
       </c>
@@ -685,7 +715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>3</v>
       </c>
@@ -693,7 +723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2</v>
       </c>
@@ -701,7 +731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>2</v>
       </c>
@@ -709,12 +739,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -814,7 +844,7 @@
       <c r="A30" s="4">
         <v>1</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="7">
         <v>1</v>
       </c>
     </row>
@@ -822,7 +852,7 @@
       <c r="A31" s="4">
         <v>2</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="7">
         <v>2</v>
       </c>
     </row>
@@ -830,7 +860,7 @@
       <c r="A32" s="4">
         <v>3</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="7">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Began mapping using Automapper
</commit_message>
<xml_diff>
--- a/docs/Favit_DataModel.xlsx
+++ b/docs/Favit_DataModel.xlsx
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,6 +584,10 @@
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>